<commit_message>
Added a new workbook for the latest test case: TC_06 - VerifyBuyer_submitsRFQtoSuppliers.
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/VerifyBuyer_submitsRFQtoSuppliers.xlsx
+++ b/src/test/resources/datasheets/VerifyBuyer_submitsRFQtoSuppliers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>BUYER</t>
   </si>
@@ -28,6 +28,24 @@
   </si>
   <si>
     <t>XEEVA -MJ</t>
+  </si>
+  <si>
+    <t>UOM</t>
+  </si>
+  <si>
+    <t>CU-CUBIC</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>supplier</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Supplier</t>
   </si>
 </sst>
 </file>
@@ -63,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,31 +378,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new test datatable,added environment,user credentials properties
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/VerifyBuyer_submitsRFQtoSuppliers.xlsx
+++ b/src/test/resources/datasheets/VerifyBuyer_submitsRFQtoSuppliers.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="15450" windowHeight="6210"/>
   </bookViews>
   <sheets>
-    <sheet name="BuyerSubmitsRFQtoSuppliers" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="BuyerSubmitsRFQtoSuppliers" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>BUYER</t>
   </si>
@@ -148,6 +148,33 @@
   </si>
   <si>
     <t>Hold;UnHold</t>
+  </si>
+  <si>
+    <t>Role2</t>
+  </si>
+  <si>
+    <t>SUPPLIER</t>
+  </si>
+  <si>
+    <t>LeadTime</t>
+  </si>
+  <si>
+    <t>FreightID</t>
+  </si>
+  <si>
+    <t>CIP</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Uprice</t>
+  </si>
+  <si>
+    <t>Uquantity</t>
   </si>
 </sst>
 </file>
@@ -183,8 +210,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,35 +507,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.42578125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -574,8 +582,23 @@
       <c r="V1" t="s">
         <v>4</v>
       </c>
+      <c r="W1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -641,6 +664,21 @@
       </c>
       <c r="V2" t="s">
         <v>5</v>
+      </c>
+      <c r="W2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -658,16 +696,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Developed new test "VerifyBuyerAwards_OR_RecommendsRFQ"
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/VerifyBuyer_submitsRFQtoSuppliers.xlsx
+++ b/src/test/resources/datasheets/VerifyBuyer_submitsRFQtoSuppliers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>BUYER</t>
   </si>
@@ -175,6 +175,24 @@
   </si>
   <si>
     <t>Uquantity</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>CurrentView</t>
+  </si>
+  <si>
+    <t>ActiveIndex</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Myview</t>
+  </si>
+  <si>
+    <t>added comments</t>
   </si>
 </sst>
 </file>
@@ -507,15 +525,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="28" max="28" width="11.28515625" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -597,8 +619,17 @@
       <c r="AA1" t="s">
         <v>47</v>
       </c>
+      <c r="AB1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:30">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -679,6 +710,15 @@
       </c>
       <c r="AA2" t="s">
         <v>48</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>